<commit_message>
Design HyperMonitorWidget and PowermaxMonitorWidget to monitor powermax model pps device data.
</commit_message>
<xml_diff>
--- a/doc/Powermax串口通信协议地址总览.xlsx
+++ b/doc/Powermax串口通信协议地址总览.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Device Version Info Registers</t>
   </si>
@@ -171,10 +171,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00：7.6m、01：15m、10：23m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[request]:010108080002EC&lt;CR&gt;&lt;LF&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -390,6 +386,14 @@
   </si>
   <si>
     <t>线圈 Coil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>割炬电缆长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00：25ft、01：50ft、10：75ft 11: 100ft</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1252,65 +1256,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1321,148 +1445,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1792,83 +1796,83 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" thickBot="1"/>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="100" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="104" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B4" s="25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="103" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B5" s="25" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="103" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B6" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="103" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B7" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="103" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B8" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="103" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B9" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="103" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="25" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="103" t="s">
+    <row r="11" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A11" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B11" s="35" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A11" s="102" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="87" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1887,7 @@
   <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F24" sqref="F24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1900,7 +1904,7 @@
     <col min="16" max="16" width="26.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.125" customWidth="1"/>
     <col min="19" max="20" width="16.375" customWidth="1"/>
-    <col min="21" max="21" width="19.375" style="88" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.375" style="36" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.25" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.125" customWidth="1"/>
     <col min="30" max="30" width="13.25" customWidth="1"/>
@@ -1921,46 +1925,46 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="95"/>
+      <c r="U1" s="42"/>
     </row>
     <row r="2" spans="1:34" ht="15">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
-      <c r="L2" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="57"/>
-      <c r="W2" s="55" t="s">
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="105"/>
+      <c r="L2" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="97"/>
+      <c r="W2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="57"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="97"/>
     </row>
     <row r="3" spans="1:34" ht="14.25" thickBot="1">
       <c r="A3" s="14" t="s">
@@ -1969,38 +1973,38 @@
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="98"/>
       <c r="L3" s="14" t="s">
         <v>5</v>
       </c>
       <c r="M3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
       <c r="P3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="96"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="99"/>
       <c r="V3" s="6"/>
       <c r="W3" s="14" t="s">
         <v>5</v>
@@ -2008,75 +2012,75 @@
       <c r="X3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" s="38" t="s">
+      <c r="Y3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="Z3" s="84"/>
+      <c r="AA3" s="84"/>
       <c r="AB3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="38" t="s">
+      <c r="AC3" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="39"/>
+      <c r="AD3" s="84"/>
+      <c r="AE3" s="84"/>
+      <c r="AF3" s="84"/>
+      <c r="AG3" s="98"/>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="17">
         <v>0</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
+      <c r="C4" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
       <c r="F4" s="17">
         <v>4</v>
       </c>
-      <c r="G4" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="49"/>
-      <c r="L4" s="97" t="s">
-        <v>78</v>
+      <c r="G4" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="102"/>
+      <c r="L4" s="43" t="s">
+        <v>77</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="52"/>
+      <c r="O4" s="89"/>
       <c r="P4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="89" t="s">
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="37" t="s">
         <v>16</v>
       </c>
       <c r="W4" s="22"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="4"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="89"/>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="52"/>
+      <c r="AC4" s="52"/>
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="89"/>
       <c r="AG4" s="19"/>
     </row>
     <row r="5" spans="1:34">
@@ -2084,51 +2088,51 @@
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45"/>
+      <c r="C5" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="50"/>
+      <c r="G5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="61"/>
       <c r="L5" s="11"/>
       <c r="M5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="52"/>
+      <c r="O5" s="89"/>
       <c r="P5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q5" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="39" t="s">
         <v>21</v>
       </c>
       <c r="V5" s="6"/>
       <c r="W5" s="22"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="45"/>
+      <c r="Z5" s="53"/>
+      <c r="AA5" s="54"/>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="51"/>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="52"/>
+      <c r="AC5" s="52"/>
+      <c r="AD5" s="90"/>
+      <c r="AE5" s="90"/>
+      <c r="AF5" s="89"/>
       <c r="AG5" s="19"/>
     </row>
     <row r="6" spans="1:34">
@@ -2136,50 +2140,50 @@
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="50"/>
+      <c r="G6" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="61"/>
       <c r="L6" s="11"/>
       <c r="M6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="N6" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="52"/>
+      <c r="O6" s="89"/>
       <c r="P6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q6" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="39" t="s">
         <v>22</v>
       </c>
       <c r="W6" s="22"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
-      <c r="Z6" s="44"/>
-      <c r="AA6" s="45"/>
+      <c r="Z6" s="53"/>
+      <c r="AA6" s="54"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="45"/>
+      <c r="AC6" s="52"/>
+      <c r="AD6" s="53"/>
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="54"/>
       <c r="AG6" s="19"/>
     </row>
     <row r="7" spans="1:34" ht="14.25" thickBot="1">
@@ -2187,51 +2191,51 @@
       <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
+      <c r="C7" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="94"/>
+      <c r="G7" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="41"/>
       <c r="L7" s="11"/>
       <c r="M7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="43" t="s">
+      <c r="N7" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="52"/>
+      <c r="O7" s="89"/>
       <c r="P7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q7" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="39" t="s">
         <v>23</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="62"/>
+      <c r="Z7" s="56"/>
+      <c r="AA7" s="57"/>
       <c r="AB7" s="13"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="61"/>
-      <c r="AE7" s="61"/>
-      <c r="AF7" s="62"/>
+      <c r="AC7" s="55"/>
+      <c r="AD7" s="56"/>
+      <c r="AE7" s="56"/>
+      <c r="AF7" s="57"/>
       <c r="AG7" s="20"/>
     </row>
     <row r="8" spans="1:34">
@@ -2239,39 +2243,39 @@
       <c r="B8" s="4">
         <v>8</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="C8" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="94"/>
+      <c r="G8" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="41"/>
       <c r="L8" s="11"/>
       <c r="M8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="N8" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="45"/>
+      <c r="O8" s="54"/>
       <c r="P8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q8" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2280,39 +2284,39 @@
       <c r="B9" s="4">
         <v>10</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
+      <c r="C9" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="G9" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="94"/>
+      <c r="G9" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="11"/>
       <c r="M9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="45"/>
-      <c r="P9" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q9" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="91" t="s">
+      <c r="O9" s="54"/>
+      <c r="P9" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q9" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="39" t="s">
         <v>27</v>
       </c>
       <c r="V9" s="2"/>
@@ -2322,35 +2326,35 @@
       <c r="B10" s="4">
         <v>12</v>
       </c>
-      <c r="C10" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
+      <c r="C10" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="94"/>
+      <c r="G10" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="41"/>
       <c r="L10" s="11"/>
       <c r="M10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="44" t="s">
+      <c r="N10" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
-      <c r="S10" s="75"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="99" t="s">
+      <c r="O10" s="54"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="45" t="s">
         <v>28</v>
       </c>
       <c r="V10" s="2"/>
@@ -2360,93 +2364,93 @@
       <c r="B11" s="4">
         <v>14</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="4">
         <v>4</v>
       </c>
-      <c r="G11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="94"/>
+      <c r="G11" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="41"/>
       <c r="L11" s="11"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="45"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="54"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="91"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="39"/>
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="11"/>
       <c r="B12" s="4">
         <v>16</v>
       </c>
-      <c r="C12" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
+      <c r="C12" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="4">
         <v>4</v>
       </c>
-      <c r="G12" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="94"/>
+      <c r="G12" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="41"/>
       <c r="L12" s="11"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="45"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="54"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="91"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="54"/>
+      <c r="U12" s="39"/>
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="11"/>
       <c r="B13" s="4">
         <v>18</v>
       </c>
-      <c r="C13" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
+      <c r="C13" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="4">
         <v>4</v>
       </c>
-      <c r="G13" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
+      <c r="G13" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="45"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="54"/>
       <c r="P13" s="5"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="91"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="39"/>
       <c r="AH13" s="2"/>
     </row>
     <row r="14" spans="1:34">
@@ -2454,110 +2458,110 @@
       <c r="B14" s="4">
         <v>20</v>
       </c>
-      <c r="C14" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
+      <c r="C14" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="4">
         <v>4</v>
       </c>
-      <c r="G14" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="50"/>
+      <c r="G14" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="61"/>
       <c r="L14" s="11"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="45"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="54"/>
       <c r="P14" s="5"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="91"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="39"/>
     </row>
     <row r="15" spans="1:34" ht="14.25" thickBot="1">
       <c r="A15" s="12"/>
       <c r="B15" s="9">
         <v>22</v>
       </c>
-      <c r="C15" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="9">
         <v>4</v>
       </c>
-      <c r="G15" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="66"/>
+      <c r="G15" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="94"/>
       <c r="L15" s="12"/>
       <c r="M15" s="34"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="98"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="62"/>
-      <c r="U15" s="92"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="40"/>
     </row>
     <row r="18" spans="1:21" ht="14.25" thickBot="1">
       <c r="L18" s="1"/>
       <c r="M18"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
-      <c r="L19" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="42"/>
+      <c r="L19" s="81" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="82"/>
+      <c r="T19" s="82"/>
+      <c r="U19" s="83"/>
     </row>
     <row r="20" spans="1:21" ht="14.25" thickBot="1">
-      <c r="A20" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="65"/>
+      <c r="A20" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="93"/>
       <c r="L20" s="14" t="s">
         <v>5</v>
       </c>
       <c r="M20" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
       <c r="P20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="Q20" s="58" t="s">
+      <c r="Q20" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="R20" s="59"/>
-      <c r="S20" s="59"/>
-      <c r="T20" s="59"/>
-      <c r="U20" s="59"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="85"/>
+      <c r="T20" s="85"/>
+      <c r="U20" s="85"/>
     </row>
     <row r="21" spans="1:21" ht="14.25" thickBot="1">
       <c r="A21" s="14" t="s">
@@ -2566,63 +2570,63 @@
       <c r="B21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="77"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="58"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="70"/>
       <c r="J21" s="23"/>
       <c r="K21" s="2"/>
       <c r="L21" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="N21" s="46" t="s">
+      <c r="N21" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="O21" s="53"/>
+      <c r="O21" s="87"/>
       <c r="P21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q21" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="89" t="s">
-        <v>59</v>
+      <c r="Q21" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="R21" s="88"/>
+      <c r="S21" s="88"/>
+      <c r="T21" s="87"/>
+      <c r="U21" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="24" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="84" t="s">
+      <c r="F22" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="78" t="s">
         <v>36</v>
       </c>
       <c r="K22" s="2"/>
@@ -2630,20 +2634,20 @@
       <c r="M22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="43" t="s">
+      <c r="N22" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="O22" s="52"/>
+      <c r="O22" s="89"/>
       <c r="P22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q22" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="90" t="s">
+      <c r="Q22" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="R22" s="90"/>
+      <c r="S22" s="90"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="38" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2657,32 +2661,32 @@
         <v>39</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="85"/>
+      <c r="F23" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="79"/>
       <c r="K23" s="2"/>
       <c r="L23" s="11"/>
       <c r="M23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N23" s="43" t="s">
+      <c r="N23" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="O23" s="52"/>
+      <c r="O23" s="89"/>
       <c r="P23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q23" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="R23" s="44"/>
-      <c r="S23" s="44"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="90" t="s">
+      <c r="Q23" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="38" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2692,24 +2696,24 @@
       <c r="C24" s="28"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="86"/>
+      <c r="F24" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="80"/>
       <c r="K24" s="2"/>
       <c r="L24" s="11"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="45"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="54"/>
       <c r="P24" s="33"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="44"/>
-      <c r="S24" s="44"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="91"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="39"/>
     </row>
     <row r="25" spans="1:21" ht="14.25" thickBot="1">
       <c r="A25" s="29"/>
@@ -2725,14 +2729,14 @@
       <c r="K25" s="2"/>
       <c r="L25" s="12"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="62"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="57"/>
       <c r="P25" s="9"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="72"/>
-      <c r="S25" s="72"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="92"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="40"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="2"/>
@@ -2753,32 +2757,49 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Q12:T12"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="Q25:T25"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="W2:AG2"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Q7:T7"/>
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:T10"/>
     <mergeCell ref="F24:I24"/>
@@ -2795,49 +2816,32 @@
     <mergeCell ref="N22:O22"/>
     <mergeCell ref="Q22:T22"/>
     <mergeCell ref="N23:O23"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="Q7:T7"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="W2:AG2"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="Q25:T25"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="Q13:T13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Design PPSInfor class to parse pps state code and fault code.
</commit_message>
<xml_diff>
--- a/doc/Powermax串口通信协议地址总览.xlsx
+++ b/doc/Powermax串口通信协议地址总览.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>Device Version Info Registers</t>
   </si>
@@ -394,6 +394,13 @@
   </si>
   <si>
     <t>00：25ft、01：50ft、10：75ft 11: 100ft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0832</t>
+  </si>
+  <si>
+    <t>气体测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1150,7 +1157,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1205,9 +1212,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1241,9 +1245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1307,15 +1308,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1325,16 +1383,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1361,9 +1419,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1401,15 +1456,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
@@ -1418,55 +1464,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1796,82 +1800,82 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" thickBot="1"/>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="44" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="49" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1887,7 +1891,7 @@
   <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:I24"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1904,7 +1908,7 @@
     <col min="16" max="16" width="26.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.125" customWidth="1"/>
     <col min="19" max="20" width="16.375" customWidth="1"/>
-    <col min="21" max="21" width="19.375" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.375" style="34" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.25" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.125" customWidth="1"/>
     <col min="30" max="30" width="13.25" customWidth="1"/>
@@ -1917,7 +1921,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="26"/>
+      <c r="M1" s="25"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -1925,46 +1929,46 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="42"/>
+      <c r="U1" s="40"/>
     </row>
     <row r="2" spans="1:34" ht="15">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="105"/>
-      <c r="L2" s="95" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
+      <c r="L2" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="97"/>
-      <c r="W2" s="95" t="s">
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="63"/>
+      <c r="W2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="96"/>
-      <c r="Y2" s="96"/>
-      <c r="Z2" s="96"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="96"/>
-      <c r="AD2" s="96"/>
-      <c r="AE2" s="96"/>
-      <c r="AF2" s="96"/>
-      <c r="AG2" s="97"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="63"/>
     </row>
     <row r="3" spans="1:34" ht="14.25" thickBot="1">
       <c r="A3" s="14" t="s">
@@ -1973,38 +1977,38 @@
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="98"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
       <c r="L3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="27" t="s">
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="70" t="s">
+      <c r="Q3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="99"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="70"/>
       <c r="V3" s="6"/>
       <c r="W3" s="14" t="s">
         <v>5</v>
@@ -2012,21 +2016,21 @@
       <c r="X3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" s="84" t="s">
+      <c r="Y3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
       <c r="AB3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="84" t="s">
+      <c r="AC3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="84"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="98"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="60"/>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" s="10" t="s">
@@ -2035,60 +2039,60 @@
       <c r="B4" s="17">
         <v>0</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="17">
         <v>4</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="102"/>
-      <c r="L4" s="43" t="s">
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="67"/>
+      <c r="L4" s="41" t="s">
         <v>77</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="89"/>
+      <c r="O4" s="52"/>
       <c r="P4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="51" t="s">
         <v>68</v>
       </c>
       <c r="R4" s="53"/>
       <c r="S4" s="53"/>
       <c r="T4" s="54"/>
-      <c r="U4" s="37" t="s">
+      <c r="U4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="22"/>
+      <c r="W4" s="21"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="4"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="89"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="52"/>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="19"/>
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="18"/>
     </row>
     <row r="5" spans="1:34">
       <c r="A5" s="11"/>
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="51" t="s">
         <v>44</v>
       </c>
       <c r="D5" s="53"/>
@@ -2096,51 +2100,51 @@
       <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="51" t="s">
         <v>45</v>
       </c>
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
-      <c r="J5" s="61"/>
+      <c r="J5" s="55"/>
       <c r="L5" s="11"/>
       <c r="M5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="89"/>
+      <c r="O5" s="52"/>
       <c r="P5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="52" t="s">
+      <c r="Q5" s="51" t="s">
         <v>69</v>
       </c>
       <c r="R5" s="53"/>
       <c r="S5" s="53"/>
       <c r="T5" s="54"/>
-      <c r="U5" s="39" t="s">
+      <c r="U5" s="37" t="s">
         <v>21</v>
       </c>
       <c r="V5" s="6"/>
-      <c r="W5" s="22"/>
+      <c r="W5" s="21"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="53"/>
       <c r="AA5" s="54"/>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="90"/>
-      <c r="AE5" s="90"/>
-      <c r="AF5" s="89"/>
-      <c r="AG5" s="19"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="52"/>
+      <c r="AG5" s="18"/>
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="11"/>
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="51" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="53"/>
@@ -2148,50 +2152,50 @@
       <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H6" s="53"/>
       <c r="I6" s="53"/>
-      <c r="J6" s="61"/>
+      <c r="J6" s="55"/>
       <c r="L6" s="11"/>
       <c r="M6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="89"/>
+      <c r="O6" s="52"/>
       <c r="P6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="52" t="s">
+      <c r="Q6" s="51" t="s">
         <v>69</v>
       </c>
       <c r="R6" s="53"/>
       <c r="S6" s="53"/>
       <c r="T6" s="54"/>
-      <c r="U6" s="39" t="s">
+      <c r="U6" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="22"/>
+      <c r="W6" s="21"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="53"/>
       <c r="AA6" s="54"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="52"/>
+      <c r="AC6" s="51"/>
       <c r="AD6" s="53"/>
       <c r="AE6" s="53"/>
       <c r="AF6" s="54"/>
-      <c r="AG6" s="19"/>
+      <c r="AG6" s="18"/>
     </row>
     <row r="7" spans="1:34" ht="14.25" thickBot="1">
       <c r="A7" s="11"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="53"/>
@@ -2199,51 +2203,51 @@
       <c r="F7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="41"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="39"/>
       <c r="L7" s="11"/>
       <c r="M7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="52" t="s">
+      <c r="N7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="89"/>
+      <c r="O7" s="52"/>
       <c r="P7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q7" s="52" t="s">
+      <c r="Q7" s="51" t="s">
         <v>72</v>
       </c>
       <c r="R7" s="53"/>
       <c r="S7" s="53"/>
       <c r="T7" s="54"/>
-      <c r="U7" s="39" t="s">
+      <c r="U7" s="37" t="s">
         <v>23</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
-      <c r="Z7" s="56"/>
-      <c r="AA7" s="57"/>
+      <c r="Z7" s="73"/>
+      <c r="AA7" s="74"/>
       <c r="AB7" s="13"/>
-      <c r="AC7" s="55"/>
-      <c r="AD7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="57"/>
-      <c r="AG7" s="20"/>
+      <c r="AC7" s="72"/>
+      <c r="AD7" s="73"/>
+      <c r="AE7" s="73"/>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="19"/>
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="11"/>
       <c r="B8" s="4">
         <v>8</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="51" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="53"/>
@@ -2251,13 +2255,13 @@
       <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="41"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="11"/>
       <c r="M8" s="4" t="s">
         <v>20</v>
@@ -2269,13 +2273,13 @@
       <c r="P8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q8" s="52" t="s">
+      <c r="Q8" s="51" t="s">
         <v>72</v>
       </c>
       <c r="R8" s="53"/>
       <c r="S8" s="53"/>
       <c r="T8" s="54"/>
-      <c r="U8" s="39" t="s">
+      <c r="U8" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2284,7 +2288,7 @@
       <c r="B9" s="4">
         <v>10</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="51" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="53"/>
@@ -2292,13 +2296,13 @@
       <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H9" s="53"/>
       <c r="I9" s="53"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="41"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="39"/>
       <c r="L9" s="11"/>
       <c r="M9" s="4" t="s">
         <v>25</v>
@@ -2307,16 +2311,16 @@
         <v>32</v>
       </c>
       <c r="O9" s="54"/>
-      <c r="P9" s="62" t="s">
+      <c r="P9" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="Q9" s="64" t="s">
+      <c r="Q9" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="39" t="s">
+      <c r="R9" s="82"/>
+      <c r="S9" s="82"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="37" t="s">
         <v>27</v>
       </c>
       <c r="V9" s="2"/>
@@ -2326,7 +2330,7 @@
       <c r="B10" s="4">
         <v>12</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="53"/>
@@ -2334,13 +2338,13 @@
       <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="53"/>
       <c r="I10" s="53"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="41"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="11"/>
       <c r="M10" s="4" t="s">
         <v>26</v>
@@ -2349,12 +2353,12 @@
         <v>33</v>
       </c>
       <c r="O10" s="54"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="68"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="45" t="s">
+      <c r="P10" s="80"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="43" t="s">
         <v>28</v>
       </c>
       <c r="V10" s="2"/>
@@ -2364,7 +2368,7 @@
       <c r="B11" s="4">
         <v>14</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="51" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="53"/>
@@ -2372,30 +2376,30 @@
       <c r="F11" s="4">
         <v>4</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H11" s="53"/>
       <c r="I11" s="53"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="41"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="39"/>
       <c r="L11" s="11"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="52"/>
+      <c r="N11" s="51"/>
       <c r="O11" s="54"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="52"/>
+      <c r="Q11" s="51"/>
       <c r="R11" s="53"/>
       <c r="S11" s="53"/>
       <c r="T11" s="54"/>
-      <c r="U11" s="39"/>
+      <c r="U11" s="37"/>
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="11"/>
       <c r="B12" s="4">
         <v>16</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="51" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="53"/>
@@ -2403,30 +2407,30 @@
       <c r="F12" s="4">
         <v>4</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="G12" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H12" s="53"/>
       <c r="I12" s="53"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="41"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="11"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="52"/>
+      <c r="N12" s="51"/>
       <c r="O12" s="54"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="52"/>
+      <c r="Q12" s="51"/>
       <c r="R12" s="53"/>
       <c r="S12" s="53"/>
       <c r="T12" s="54"/>
-      <c r="U12" s="39"/>
+      <c r="U12" s="37"/>
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="11"/>
       <c r="B13" s="4">
         <v>18</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="51" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="53"/>
@@ -2434,23 +2438,23 @@
       <c r="F13" s="4">
         <v>4</v>
       </c>
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H13" s="53"/>
       <c r="I13" s="53"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="52"/>
+      <c r="N13" s="51"/>
       <c r="O13" s="54"/>
       <c r="P13" s="5"/>
-      <c r="Q13" s="52"/>
+      <c r="Q13" s="51"/>
       <c r="R13" s="53"/>
       <c r="S13" s="53"/>
       <c r="T13" s="54"/>
-      <c r="U13" s="39"/>
+      <c r="U13" s="37"/>
       <c r="AH13" s="2"/>
     </row>
     <row r="14" spans="1:34">
@@ -2458,7 +2462,7 @@
       <c r="B14" s="4">
         <v>20</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="53"/>
@@ -2466,102 +2470,102 @@
       <c r="F14" s="4">
         <v>4</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="51" t="s">
         <v>47</v>
       </c>
       <c r="H14" s="53"/>
       <c r="I14" s="53"/>
-      <c r="J14" s="61"/>
+      <c r="J14" s="55"/>
       <c r="L14" s="11"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="52"/>
+      <c r="N14" s="51"/>
       <c r="O14" s="54"/>
       <c r="P14" s="5"/>
-      <c r="Q14" s="52"/>
+      <c r="Q14" s="51"/>
       <c r="R14" s="53"/>
       <c r="S14" s="53"/>
       <c r="T14" s="54"/>
-      <c r="U14" s="39"/>
+      <c r="U14" s="37"/>
     </row>
     <row r="15" spans="1:34" ht="14.25" thickBot="1">
       <c r="A15" s="12"/>
       <c r="B15" s="9">
         <v>22</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="74"/>
       <c r="F15" s="9">
         <v>4</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="94"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="78"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="57"/>
-      <c r="U15" s="40"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="38"/>
     </row>
     <row r="18" spans="1:21" ht="14.25" thickBot="1">
       <c r="L18" s="1"/>
       <c r="M18"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
-      <c r="L19" s="81" t="s">
+      <c r="L19" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="82"/>
-      <c r="S19" s="82"/>
-      <c r="T19" s="82"/>
-      <c r="U19" s="83"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="98"/>
+      <c r="R19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
+      <c r="U19" s="99"/>
     </row>
     <row r="20" spans="1:21" ht="14.25" thickBot="1">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="93"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="77"/>
       <c r="L20" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="27" t="s">
+      <c r="M20" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="N20" s="84"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="27" t="s">
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="Q20" s="70" t="s">
+      <c r="Q20" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="R20" s="85"/>
-      <c r="S20" s="85"/>
-      <c r="T20" s="85"/>
-      <c r="U20" s="85"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="69"/>
     </row>
     <row r="21" spans="1:21" ht="14.25" thickBot="1">
       <c r="A21" s="14" t="s">
@@ -2570,41 +2574,41 @@
       <c r="B21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="71"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="84" t="s">
+      <c r="F21" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="23"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="22"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="20" t="s">
         <v>75</v>
       </c>
       <c r="M21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="N21" s="86" t="s">
+      <c r="N21" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="O21" s="87"/>
+      <c r="O21" s="100"/>
       <c r="P21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="Q21" s="86" t="s">
+      <c r="Q21" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="R21" s="88"/>
-      <c r="S21" s="88"/>
-      <c r="T21" s="87"/>
-      <c r="U21" s="37" t="s">
+      <c r="R21" s="101"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="35" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2616,17 +2620,17 @@
         <v>37</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="23" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="78" t="s">
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="94" t="s">
         <v>36</v>
       </c>
       <c r="K22" s="2"/>
@@ -2634,20 +2638,20 @@
       <c r="M22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="52" t="s">
+      <c r="N22" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="O22" s="89"/>
+      <c r="O22" s="52"/>
       <c r="P22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q22" s="52" t="s">
+      <c r="Q22" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="89"/>
-      <c r="U22" s="38" t="s">
+      <c r="R22" s="71"/>
+      <c r="S22" s="71"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2661,82 +2665,86 @@
         <v>39</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="79"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="95"/>
       <c r="K23" s="2"/>
       <c r="L23" s="11"/>
       <c r="M23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N23" s="52" t="s">
+      <c r="N23" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="O23" s="89"/>
+      <c r="O23" s="52"/>
       <c r="P23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Q23" s="52" t="s">
+      <c r="Q23" s="51" t="s">
         <v>62</v>
       </c>
       <c r="R23" s="53"/>
       <c r="S23" s="53"/>
       <c r="T23" s="54"/>
-      <c r="U23" s="38" t="s">
+      <c r="U23" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="11"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="80"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="96"/>
       <c r="K24" s="2"/>
       <c r="L24" s="11"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="52"/>
+      <c r="N24" s="51"/>
       <c r="O24" s="54"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="52"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="51"/>
       <c r="R24" s="53"/>
       <c r="S24" s="53"/>
       <c r="T24" s="54"/>
-      <c r="U24" s="39"/>
+      <c r="U24" s="37"/>
     </row>
     <row r="25" spans="1:21" ht="14.25" thickBot="1">
-      <c r="A25" s="29"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="13"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="E25" s="13"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="29"/>
       <c r="K25" s="2"/>
       <c r="L25" s="12"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="57"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="74"/>
       <c r="P25" s="9"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="40"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="103"/>
+      <c r="S25" s="103"/>
+      <c r="T25" s="104"/>
+      <c r="U25" s="38"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="2"/>
@@ -2756,50 +2764,27 @@
       <c r="J29" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="L2:U2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="W2:AG2"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="Q7:T7"/>
+  <mergeCells count="86">
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="Q25:T25"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:T10"/>
     <mergeCell ref="F24:I24"/>
@@ -2816,6 +2801,22 @@
     <mergeCell ref="N22:O22"/>
     <mergeCell ref="Q22:T22"/>
     <mergeCell ref="N23:O23"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C12:E12"/>
@@ -2823,25 +2824,33 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="Q25:T25"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Q12:T12"/>
-    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="W2:AG2"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>